<commit_message>
Marcar presença - folha 14: A, B, C, D, E
</commit_message>
<xml_diff>
--- a/docs/attendance.xlsx
+++ b/docs/attendance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Attendance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\attendance-backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,14 +19,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Migração!$A$1:$G$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Módulos!$B$2:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Projetos!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Projetos!$B$2:$E$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="73">
   <si>
     <t>Seq.</t>
   </si>
@@ -165,33 +165,9 @@
     <t>Star</t>
   </si>
   <si>
-    <t xml:space="preserve">        Migrar 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Migrar 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Migrar 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Migrar 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Migrar 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Migrar 2008</t>
-  </si>
-  <si>
     <t>Projeto</t>
   </si>
   <si>
-    <t>Integração de tags (Biderecional?)</t>
-  </si>
-  <si>
-    <t>Gerar resumo sr</t>
-  </si>
-  <si>
     <t>Heroku - QuickStart</t>
   </si>
   <si>
@@ -199,6 +175,78 @@
   </si>
   <si>
     <t>Springboot 9 Guides (3/dia)</t>
+  </si>
+  <si>
+    <t>Migrar 2014</t>
+  </si>
+  <si>
+    <t>Migrar 2013</t>
+  </si>
+  <si>
+    <t>Migrar 2012</t>
+  </si>
+  <si>
+    <t>Migrar 2010</t>
+  </si>
+  <si>
+    <t>Migrar 2009</t>
+  </si>
+  <si>
+    <t>Migrar 2008</t>
+  </si>
+  <si>
+    <t>WhatApp</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Resumo sr E6 query etc</t>
+  </si>
+  <si>
+    <t>Dashboard - indicadores do labor</t>
+  </si>
+  <si>
+    <t>Manter contatos - admin</t>
+  </si>
+  <si>
+    <t>Ficha de cadastro publica (pág. 12)</t>
+  </si>
+  <si>
+    <t>Ficha de cadastro papel (pág. 12)</t>
+  </si>
+  <si>
+    <t>Período</t>
+  </si>
+  <si>
+    <t>1º semestre 2017</t>
+  </si>
+  <si>
+    <t>Marcar presenças</t>
+  </si>
+  <si>
+    <t>Migrar 2017 usando App</t>
+  </si>
+  <si>
+    <t>Migrar meses 2016 ausentes usando App</t>
+  </si>
+  <si>
+    <t>Atenticação e autorização</t>
+  </si>
+  <si>
+    <t>Conclusão</t>
+  </si>
+  <si>
+    <t>data...</t>
+  </si>
+  <si>
+    <t>Início</t>
+  </si>
+  <si>
+    <t>Upload foto: crud person, ficha pública</t>
+  </si>
+  <si>
+    <t>Upload foto: integração google contatos, outros</t>
   </si>
 </sst>
 </file>
@@ -232,7 +280,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -345,429 +399,506 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -808,8 +939,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="37"/>
-      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="wholeTable" dxfId="43"/>
+      <tableStyleElement type="headerRow" dxfId="42"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1110,17 +1241,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.75" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1141,7 +1272,7 @@
       <c r="C3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1152,222 +1283,244 @@
       <c r="C4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2">
+        <v>31</v>
+      </c>
+      <c r="D5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2">
+        <v>32</v>
+      </c>
+      <c r="D6" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2">
+        <v>20</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D11" s="22"/>
     </row>
     <row r="12" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D12" s="22"/>
     </row>
     <row r="13" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D14" s="22"/>
     </row>
     <row r="15" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D15" s="22"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="D16" s="22"/>
     </row>
     <row r="17" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="D18" s="22"/>
     </row>
     <row r="19" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="D20" s="22"/>
     </row>
     <row r="21" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D21" s="22"/>
     </row>
     <row r="22" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D23" s="22"/>
     </row>
     <row r="24" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="D24" s="22"/>
     </row>
     <row r="25" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
+        <v>23</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
         <v>24</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C27" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D27" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:D2">
-    <sortState ref="B3:D26">
+    <sortState ref="B3:D27">
       <sortCondition ref="D2"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="D3:D27">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+      <formula>"~"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+      <formula>"n/a"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1375,172 +1528,437 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="B2:G25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.875" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.75" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="2" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="str">
+        <f>IF(C3="","",VLOOKUP(C3,Módulos!B:C,2,FALSE))</f>
+        <v>Backend - REST</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="26">
+        <v>42845</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="str">
+        <f>IF(C4="","",VLOOKUP(C4,Módulos!B:C,2,FALSE))</f>
+        <v>Backend - REST</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="22">
+        <v>2</v>
+      </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="str">
+        <f>IF(C5="","",VLOOKUP(C5,Módulos!B:C,2,FALSE))</f>
+        <v>Front - Web</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="22">
+        <v>3</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="str">
+        <f>IF(C6="","",VLOOKUP(C6,Módulos!B:C,2,FALSE))</f>
+        <v>API - Dropbox</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="22">
+        <v>4</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="str">
+        <f>IF(C7="","",VLOOKUP(C7,Módulos!B:C,2,FALSE))</f>
+        <v>Ficha de cadastro</v>
+      </c>
+      <c r="C7" s="2">
+        <v>13</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="22">
+        <v>5</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="str">
+        <f>IF(C8="","",VLOOKUP(C8,Módulos!B:C,2,FALSE))</f>
+        <v>Backend - REST</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="22">
+        <v>6</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="str">
+        <f>IF(C9="","",VLOOKUP(C9,Módulos!B:C,2,FALSE))</f>
+        <v>Página de cadastro inteligente</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="22">
+        <v>7</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="str">
+        <f>IF(C10="","",VLOOKUP(C10,Módulos!B:C,2,FALSE))</f>
+        <v>Tableau</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="22">
+        <v>8</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="str">
+        <f>IF(C11="","",VLOOKUP(C11,Módulos!B:C,2,FALSE))</f>
+        <v>Front - Web</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="22">
+        <v>9</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="str">
+        <f>IF(C12="","",VLOOKUP(C12,Módulos!B:C,2,FALSE))</f>
+        <v>Backend - REST</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="str">
+        <f>IF(C13="","",VLOOKUP(C13,Módulos!B:C,2,FALSE))</f>
+        <v>Backend - REST</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="str">
+        <f>IF(C14="","",VLOOKUP(C14,Módulos!B:C,2,FALSE))</f>
+        <v>Backend - REST</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="str">
+        <f>IF(C15="","",VLOOKUP(C15,Módulos!B:C,2,FALSE))</f>
+        <v>DB</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="str">
+        <f>IF(C16="","",VLOOKUP(C16,Módulos!B:C,2,FALSE))</f>
+        <v>DB</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="str">
+        <f>IF(C17="","",VLOOKUP(C17,Módulos!B:C,2,FALSE))</f>
+        <v>DB</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="E17" s="22"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="23" t="str">
+        <f>IF(C18="","",VLOOKUP(C18,Módulos!B:C,2,FALSE))</f>
+        <v>DB</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="23" t="str">
+        <f>IF(C19="","",VLOOKUP(C19,Módulos!B:C,2,FALSE))</f>
+        <v>DB</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="str">
+        <f>IF(C20="","",VLOOKUP(C20,Módulos!B:C,2,FALSE))</f>
+        <v>DB</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="str">
+        <f>IF(C21="","",VLOOKUP(C21,Módulos!B:C,2,FALSE))</f>
+        <v>Página de cadastro inteligente</v>
+      </c>
+      <c r="C21" s="2">
+        <v>12</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="23" t="str">
+        <f>IF(C22="","",VLOOKUP(C22,Módulos!B:C,2,FALSE))</f>
+        <v>API - Google Contatcs</v>
+      </c>
+      <c r="C22" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="D22" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="23" t="str">
+        <f>IF(C23="","",VLOOKUP(C23,Módulos!B:C,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="23" t="str">
+        <f>IF(C24="","",VLOOKUP(C24,Módulos!B:C,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="23" t="str">
+        <f>IF(C25="","",VLOOKUP(C25,Módulos!B:C,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1">
-    <sortState ref="A2:C25">
-      <sortCondition ref="B1"/>
+  <autoFilter ref="B2:E2">
+    <sortState ref="B3:E25">
+      <sortCondition ref="E2"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="E4:E25">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+      <formula>"ok"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+      <formula>"~"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+      <formula>"n/a"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1555,15 +1973,15 @@
       <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="11.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">

</xml_diff>